<commit_message>
Update 8. Harmonising standards/Harmonizing SXI-DF.xlsx
added SXI options
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/Harmonizing SXI-DF.xlsx
+++ b/8. Harmonising standards/Harmonizing SXI-DF.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gta\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sxDaten\GitHub\DataFactory-Knowledge-Center\8. Harmonising standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5293ED0E-6CB2-47DD-8237-F30E75204597}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEEC653-5C2C-4941-99FB-21E6BA2EFA32}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15840" xr2:uid="{16C57660-5F26-45F7-8E47-1B4877DEBD5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Zielstellung" sheetId="2" r:id="rId1"/>
     <sheet name="Datenstruktur" sheetId="1" r:id="rId2"/>
+    <sheet name="Prozess" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Vertrieblich</t>
   </si>
@@ -64,6 +65,36 @@
   </si>
   <si>
     <t>Modellierung und Saldenlistenimport erfordert DataFactory</t>
+  </si>
+  <si>
+    <t>Download SXI Logik als XML Dateien möglich</t>
+  </si>
+  <si>
+    <t>NVARCHAR muss in SXI eingestellt werden</t>
+  </si>
+  <si>
+    <t>Upload von geänderten Dateien pro Kunde mit Versionierung</t>
+  </si>
+  <si>
+    <t>Besser create Script für Datenbank für flexible Tabellendefinition ?</t>
+  </si>
+  <si>
+    <t>Webserver Yeti läuft als Dienst auf Port 8089</t>
+  </si>
+  <si>
+    <t>Vadin generiert HTML Seiten</t>
+  </si>
+  <si>
+    <t>Jenkins, Nexus, Maeven für Build -&gt; auf Azure verfügbar - in VM, Container, Service ?</t>
+  </si>
+  <si>
+    <t>Repo im Stash auf Azure</t>
+  </si>
+  <si>
+    <t>Beispiel Greif Velux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">willl Power BI für PSI Penta, </t>
   </si>
 </sst>
 </file>
@@ -5460,10 +5491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57257774-D818-4A13-91F1-A7DCB0C009FC}">
-  <dimension ref="B2:N45"/>
+  <dimension ref="B2:N51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5520,6 +5551,16 @@
         <v>9</v>
       </c>
     </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5540,4 +5581,59 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71006EA9-40F6-4D3A-95DF-25D6B75326D9}">
+  <dimension ref="B4:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modelllierung ergänzt, alle Abrechnungsübersichten gelöscht
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/Harmonizing SXI-DF.xlsx
+++ b/8. Harmonising standards/Harmonizing SXI-DF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DataFactory-Knowledge-Center\8. Harmonising standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB1AFDB-4938-4236-A182-6E41CBCC735F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D3D1B3-9A18-4E4F-99F1-D4D7549C892B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15840" xr2:uid="{16C57660-5F26-45F7-8E47-1B4877DEBD5B}"/>
   </bookViews>
@@ -1655,15 +1655,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>676275</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1678,8 +1678,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5781675" y="3362325"/>
-          <a:ext cx="5886450" cy="390525"/>
+          <a:off x="5724525" y="3228975"/>
+          <a:ext cx="5886450" cy="781050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1722,6 +1722,53 @@
             </a:rPr>
             <a:t>Modellierung</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Attribute</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> an Knoten (Stammkostenstelle)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Zeitabhängige Modellierung (IC Kennzeichen)</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="lt1"/>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr marL="0" indent="0" algn="ctr"/>
@@ -2274,15 +2321,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>380999</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2297,7 +2344,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5791200" y="3819525"/>
+          <a:off x="5724525" y="4048125"/>
           <a:ext cx="1771649" cy="1152525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2491,15 +2538,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>666749</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>619124</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2514,7 +2561,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7600950" y="3819525"/>
+          <a:off x="7553325" y="4048125"/>
           <a:ext cx="1771649" cy="1152525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2649,15 +2696,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2672,7 +2719,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9439275" y="3819525"/>
+          <a:off x="9382125" y="4038600"/>
           <a:ext cx="2257425" cy="1152525"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3047,13 +3094,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>521493</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
@@ -3072,9 +3119,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="8465343" y="4972050"/>
-          <a:ext cx="21432" cy="409575"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8439150" y="5200650"/>
+          <a:ext cx="26193" cy="180975"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -6901,7 +6948,7 @@
   <dimension ref="B2:N63"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q36" sqref="Q36"/>
+      <selection activeCell="S23" sqref="S23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update konzept nach Gespräch mit Stanislav
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/Harmonizing SXI-DF.xlsx
+++ b/8. Harmonising standards/Harmonizing SXI-DF.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DataFactory-Knowledge-Center\8. Harmonising standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE17F8A-3D78-4454-8F28-A39F860162BB}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76193A37-73CD-4E22-B410-AAD5D5891E94}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15840" activeTab="6" xr2:uid="{16C57660-5F26-45F7-8E47-1B4877DEBD5B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{16C57660-5F26-45F7-8E47-1B4877DEBD5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Zielstellung_BigBigPicture" sheetId="6" r:id="rId1"/>
-    <sheet name="Zielstellung_BigPicture" sheetId="4" r:id="rId2"/>
-    <sheet name="Zielstellung_Detail" sheetId="2" r:id="rId3"/>
-    <sheet name="Rollen" sheetId="5" r:id="rId4"/>
+    <sheet name="Rollen" sheetId="5" r:id="rId2"/>
+    <sheet name="Zielstellung_BigPicture" sheetId="4" r:id="rId3"/>
+    <sheet name="Zielstellung_Detail" sheetId="2" r:id="rId4"/>
     <sheet name="Datenstruktur" sheetId="1" r:id="rId5"/>
     <sheet name="Prozess" sheetId="3" r:id="rId6"/>
     <sheet name="Betriebsoptionen" sheetId="7" r:id="rId7"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
   <si>
     <t>Technisch</t>
   </si>
@@ -189,61 +189,10 @@
     <t>Methodenkompetenz - die richtigen Tools bauen und einsetzen</t>
   </si>
   <si>
-    <t>Softwarearchitektur</t>
-  </si>
-  <si>
-    <t>Rollen Tool</t>
-  </si>
-  <si>
-    <t>Rollen Prozess</t>
-  </si>
-  <si>
-    <t>Vertrieb</t>
-  </si>
-  <si>
-    <t>Lehre</t>
-  </si>
-  <si>
-    <t>Prozessmethodik</t>
-  </si>
-  <si>
     <t>Projektcontrolling</t>
   </si>
   <si>
     <t>Datenintegration</t>
-  </si>
-  <si>
-    <t>Planung</t>
-  </si>
-  <si>
-    <t>Verwaltung</t>
-  </si>
-  <si>
-    <t>Entwicklung Integrationsplattform</t>
-  </si>
-  <si>
-    <t>Entwicklung Planungsplattform</t>
-  </si>
-  <si>
-    <t>Entwicklung Integrationsmodule</t>
-  </si>
-  <si>
-    <t>Entwicklung Planungsmodule</t>
-  </si>
-  <si>
-    <t>Entwicklung Visualisierung, Modellierung</t>
-  </si>
-  <si>
-    <t>Rollen Lösungen</t>
-  </si>
-  <si>
-    <t>Entwicklung Visualisierungsmodule</t>
-  </si>
-  <si>
-    <t>QS</t>
-  </si>
-  <si>
-    <t>Support</t>
   </si>
   <si>
     <t>Geben Ihnen Überblick und Transparenz indem wir alle Ihre Datenquellen in einem Datawarehouse integrieren.</t>
@@ -279,15 +228,6 @@
     <t>Starke eigene Platzierung und gleichzeitig ein gefragter Partner</t>
   </si>
   <si>
-    <t>Mitarbeiter mit einem Schwerpunkt und einem integrierten Thema</t>
-  </si>
-  <si>
-    <t>Arne - Personaldatenintegration und Personalplanung</t>
-  </si>
-  <si>
-    <t>Toni - Datenintegration und Zusatzbuchungsjournale</t>
-  </si>
-  <si>
     <t>Direktaufgaben welche länger als 2 Monate offen sind (Abrechnung vergessen)</t>
   </si>
   <si>
@@ -298,15 +238,6 @@
   </si>
   <si>
     <t>Projekte mit außergewöhnlichem Zeitaufwand und geringem Ertrag</t>
-  </si>
-  <si>
-    <t>Mitarbeiter mit Organisationsaufgabe</t>
-  </si>
-  <si>
-    <t>Prozessorganisation</t>
-  </si>
-  <si>
-    <t>Solutionentwicklung</t>
   </si>
   <si>
     <t>PowerBI / Qlikmuster</t>
@@ -333,9 +264,6 @@
     <t>Rechtesystem</t>
   </si>
   <si>
-    <t>Referenzprojekte</t>
-  </si>
-  <si>
     <t>SFZ Chemnitz</t>
   </si>
   <si>
@@ -355,6 +283,12 @@
   </si>
   <si>
     <t>Alle drei Bausteine können einzeln eingesetzt werden.</t>
+  </si>
+  <si>
+    <t>Sollten mehrere Rollen in der Firma besetzten</t>
+  </si>
+  <si>
+    <t>Referenzprojekte für Etablierung</t>
   </si>
 </sst>
 </file>
@@ -1609,6 +1543,2945 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>147638</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>109538</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rechteck 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0542BCD-E529-4121-AFCC-13793B6A2DA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3181350" y="7748588"/>
+          <a:ext cx="890588" cy="519113"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>IST</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>742951</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>109539</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rechteck 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6FE837FA-CE56-47E4-A5AA-5D0827857286}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3181351" y="7072312"/>
+          <a:ext cx="890588" cy="519113"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>PLAN</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>109538</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rechteck 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C98810BA-DEC4-41A2-B374-4396B9BDDE17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3181350" y="6381749"/>
+          <a:ext cx="890588" cy="519113"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>VISU</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>500062</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Textfeld 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C60522C8-AD92-421C-AD47-5E3878DA70FB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2981325" y="5934074"/>
+          <a:ext cx="1481137" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>Softwareentwicklung</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>61913</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Textfeld 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65664833-6939-4F9E-8528-99E4F5F8DEF2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4786313" y="5934074"/>
+          <a:ext cx="1481137" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>Modulentwicklung</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>52388</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Textfeld 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10CF2FF6-879C-426C-83E1-CD42BB2F17C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4014788" y="5505449"/>
+          <a:ext cx="1481137" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>Produkt</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>585788</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>90486</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>147636</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Textfeld 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E3F9142-9A13-451E-99A3-990615FFA70B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7596188" y="5519736"/>
+          <a:ext cx="1481137" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Prozess</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>733426</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>104777</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>109538</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rechteck 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAB192DE-9E08-496F-90CD-C7E383E7FF61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3171826" y="8429627"/>
+          <a:ext cx="900112" cy="295274"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>QS</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>752476</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>14290</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>128588</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>128589</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rechteck 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E969C3D-137A-47DF-A9E2-11B582645B01}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3190876" y="8882065"/>
+          <a:ext cx="900112" cy="295274"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Handbuch</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>538163</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>290513</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Rechteck 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97920A63-7A93-4337-8FF5-19D9C834C093}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4500563" y="7948613"/>
+          <a:ext cx="514350" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>I1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>457201</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>176213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rechteck 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2673E709-FCDA-475A-AA98-3D3A60217941}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5181601" y="7958138"/>
+          <a:ext cx="514350" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>I2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>433389</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>185739</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Rechteck 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F61A05C1-5370-4C4B-AFDE-C3DCD5E0C9EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5919789" y="7943850"/>
+          <a:ext cx="514350" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>I3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>509588</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>147639</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>261938</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>123827</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Rechteck 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5D71E5F-D801-4068-A5CF-A2634C9D105A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4471988" y="7205664"/>
+          <a:ext cx="514350" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>P1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>457201</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>147639</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>123827</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Rechteck 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{820D05F2-9C5B-400B-B4E5-9D25EF5F3EFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5181601" y="7205664"/>
+          <a:ext cx="514350" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>P2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>147639</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>123827</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rechteck 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{053C2800-3089-4CDE-A56D-D2CEF2542DC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5934075" y="7205664"/>
+          <a:ext cx="514350" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>P3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>23814</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Rechteck 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3663CE14-3648-4605-B9E1-53E5DCD935FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4448175" y="6538914"/>
+          <a:ext cx="514350" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>V1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>481012</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>23814</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>233362</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Rechteck 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AFCBA409-6311-417B-BEF9-C1DDCE5B9686}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5205412" y="6538914"/>
+          <a:ext cx="514350" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>V2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>23814</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Rechteck 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D010A1E9-FB2B-4EEF-8298-DDD1B14C7F43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5934075" y="6538914"/>
+          <a:ext cx="514350" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>V3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>357188</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>347663</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Rechteck 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C01BA4C-A3B8-4C9C-8437-E847579159D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5081588" y="6429375"/>
+          <a:ext cx="752475" cy="1981200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>366713</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>128586</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>4761</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Textfeld 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFAA47A8-BD28-4605-BD33-68C918C66AD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5091113" y="8453436"/>
+          <a:ext cx="833437" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Solution</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>61914</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38102</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Rechteck 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84CAAB2F-AE51-45E0-956E-BE3648CC7E3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8062912" y="8567739"/>
+          <a:ext cx="862013" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Vertrieb</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>290512</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>42864</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Rechteck 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E48B398F-410C-47C6-A013-B1DA2AD70544}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8062912" y="8029576"/>
+          <a:ext cx="862013" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Konzeption</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276224</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>128589</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>376237</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>104777</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Rechteck 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B3DA40C-2FE2-4A46-BB06-CC73D7047811}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8048624" y="7548564"/>
+          <a:ext cx="862013" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Integration</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>42864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>357187</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19052</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Rechteck 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{12C66A82-5E00-4C81-B213-DD9462258C16}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8029574" y="7100889"/>
+          <a:ext cx="862013" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Planung</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>257174</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>95252</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>357187</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>71440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Rechteck 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD1B937C-4938-4AB0-A3BD-7FB1FEDA5AD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8029574" y="6610352"/>
+          <a:ext cx="862013" cy="338138"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Visual</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>661988</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>61914</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Rechteck 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBFFE0BE-5E99-4EF0-97F0-50DB2DDEEC3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9196388" y="8205789"/>
+          <a:ext cx="976312" cy="438149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Projekt-controlling</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>90487</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="Rechteck 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C14228D-63F7-4350-A691-54E01B45C5C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9182100" y="7305675"/>
+          <a:ext cx="966787" cy="438149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Prozess-organisation</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>133352</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>166687</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>109538</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Rechteck 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B816D6E-2900-4BCF-BAC2-9479DDD9DA32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7077074" y="7372352"/>
+          <a:ext cx="862013" cy="519111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Projekt-leitung</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Rechteck 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94E347C1-7FBB-459C-A779-2B205BF90048}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7015163" y="10610850"/>
+          <a:ext cx="966787" cy="438149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Verwaltung</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>385764</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590551</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Rechteck 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{181C629B-3D1F-44E7-BE2B-1EFDB8E12776}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5872164" y="10610851"/>
+          <a:ext cx="966787" cy="438149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>IT</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304801</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>90490</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>442913</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>23814</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Rechteck 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF218DAC-C9B5-440B-BCD3-D704D9D81279}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5029201" y="9320215"/>
+          <a:ext cx="900112" cy="295274"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Support</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>690563</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>214313</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Textfeld 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C600075A-BE29-4994-99D4-E45BE4FC6A20}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11510963" y="6572249"/>
+          <a:ext cx="2571750" cy="742952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Wir wollen Projekte</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> ohne Dienstleistung oder mit sehr viel Dienstleistung - aber möglichst nicht in der Mitte.</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>109538</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>119063</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Textfeld 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C3D7E9C-A156-4D23-A7B2-FD71AB7C23B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7881938" y="5829299"/>
+          <a:ext cx="1347787" cy="261939"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>10-50 Tage Projekt</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>757238</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>95253</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>28577</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Rechteck 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CD74041-74D2-4D22-8132-E0BB9322B387}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3195638" y="9324978"/>
+          <a:ext cx="900112" cy="295274"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Schulung</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>385763</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Rechteck 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F01D846F-5910-4427-938E-8B142FCEE9A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8048626" y="9267826"/>
+          <a:ext cx="871537" cy="438149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Betrieb</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>138113</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>614363</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>171451</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Gerader Verbinder 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5187FE38-96C3-4368-9BB9-6B6DA8BDFC19}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6858000" y="5567363"/>
+          <a:ext cx="4763" cy="4195763"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>366713</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Gerader Verbinder 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{694E555F-CFE2-4749-88EA-4C51827080F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3200400" y="9991725"/>
+          <a:ext cx="7986713" cy="47625"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="15875">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>728662</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="Textfeld 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76BB8D43-F3D6-41CA-B5AC-B911ABF271DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6257925" y="10163174"/>
+          <a:ext cx="1481137" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1400" b="1"/>
+            <a:t>Infrastruktur</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>133351</xdr:colOff>
       <xdr:row>16</xdr:row>
@@ -3011,7 +5884,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6328,7 +9201,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -9380,7 +12253,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10943,7 +13816,7 @@
   <dimension ref="B2:N49"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10961,47 +13834,47 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B5" s="1" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="E9" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
-        <v>92</v>
+        <v>69</v>
       </c>
       <c r="E11" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.45">
       <c r="H19" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.45">
@@ -11016,6 +13889,93 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28EF74D8-9026-466E-B120-5AD0A17FB84D}">
+  <dimension ref="B2:M14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="K12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+      <c r="K13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE61C21-B4DF-4ACF-89E3-F75BA53700E1}">
   <dimension ref="B2:N49"/>
   <sheetViews>
@@ -11033,52 +13993,52 @@
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="L3" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="L4" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.45">
@@ -11092,7 +14052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57257774-D818-4A13-91F1-A7DCB0C009FC}">
   <dimension ref="B2:N63"/>
   <sheetViews>
@@ -11141,17 +14101,17 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="N9" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="N10" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.45">
       <c r="N11" t="s">
-        <v>106</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.45">
@@ -11215,189 +14175,6 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28EF74D8-9026-466E-B120-5AD0A17FB84D}">
-  <dimension ref="B2:N28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="2.1328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B2" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="M3" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B4" t="s">
-        <v>49</v>
-      </c>
-      <c r="M4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="M5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="M7" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
-        <v>51</v>
-      </c>
-      <c r="N8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="N9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="N10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
-        <v>52</v>
-      </c>
-      <c r="J14" t="s">
-        <v>55</v>
-      </c>
-      <c r="M14" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="N15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F16" t="s">
-        <v>64</v>
-      </c>
-      <c r="J16" t="s">
-        <v>60</v>
-      </c>
-      <c r="N16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="N17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" t="s">
-        <v>65</v>
-      </c>
-      <c r="J18" t="s">
-        <v>59</v>
-      </c>
-      <c r="N18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F20" t="s">
-        <v>68</v>
-      </c>
-      <c r="J20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" t="s">
-        <v>69</v>
-      </c>
-      <c r="J22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="J24" t="s">
-        <v>58</v>
-      </c>
-      <c r="M24" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="N25" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="J26" t="s">
-        <v>70</v>
-      </c>
-      <c r="N26" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="N27" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.45">
-      <c r="J28" t="s">
-        <v>61</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11583,8 +14360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DACF6E-0F61-4744-BDED-4D535B825F26}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Überlegungen mit aus Meeting / mit Stefan
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/Harmonizing SXI-DF.xlsx
+++ b/8. Harmonising standards/Harmonizing SXI-DF.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DataFactory-Knowledge-Center\8. Harmonising standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33BA9D7-8C6A-4556-A681-5413843E1728}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B3B10B-BD9A-4ED7-A70B-397C1B760287}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{16C57660-5F26-45F7-8E47-1B4877DEBD5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Zielstellung_BigBigPicture" sheetId="6" r:id="rId1"/>
     <sheet name="Rollen" sheetId="5" r:id="rId2"/>
-    <sheet name="Zielstellung_BigPicture" sheetId="4" r:id="rId3"/>
-    <sheet name="Zielstellung_Detail" sheetId="2" r:id="rId4"/>
-    <sheet name="Datenstruktur" sheetId="1" r:id="rId5"/>
-    <sheet name="Prozess" sheetId="3" r:id="rId6"/>
-    <sheet name="Betriebsoptionen" sheetId="7" r:id="rId7"/>
+    <sheet name="Schritte" sheetId="8" r:id="rId3"/>
+    <sheet name="Zielstellung_BigPicture" sheetId="4" r:id="rId4"/>
+    <sheet name="Zielstellung_Detail" sheetId="2" r:id="rId5"/>
+    <sheet name="Datenstruktur" sheetId="1" r:id="rId6"/>
+    <sheet name="Prozess" sheetId="3" r:id="rId7"/>
+    <sheet name="Betriebsoptionen" sheetId="7" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="136">
   <si>
     <t>Technisch</t>
   </si>
@@ -202,9 +203,6 @@
   </si>
   <si>
     <t>Ermöglichen Ihnen sehr viele Mitarbeiter im Unternehmen auf sehr einfache Weise einzubeziehen.</t>
-  </si>
-  <si>
-    <t>Plattform zur Unternehmensführung - Integration von Daten, Personen und Ideen</t>
   </si>
   <si>
     <t>tagesaktuelle Datenintegration</t>
@@ -395,12 +393,60 @@
   <si>
     <t>Hügel zum U machen</t>
   </si>
+  <si>
+    <t>DB Meeting mit Definition Solution Kontoplan</t>
+  </si>
+  <si>
+    <t>SXI Schemaanpassung</t>
+  </si>
+  <si>
+    <t>Primärschlüssel</t>
+  </si>
+  <si>
+    <t>Regeln für Datentypen</t>
+  </si>
+  <si>
+    <t>Konfigurationsservice</t>
+  </si>
+  <si>
+    <t>Download</t>
+  </si>
+  <si>
+    <t>Visualisierung</t>
+  </si>
+  <si>
+    <t>Developer Meeting mit Mike</t>
+  </si>
+  <si>
+    <t>Modulare Plattform für Unternehmensführung - Integration von Daten, Personen und Ideen</t>
+  </si>
+  <si>
+    <t>MOPLUF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modulare Plattform für </t>
+  </si>
+  <si>
+    <t>Daten</t>
+  </si>
+  <si>
+    <t>Lösungen</t>
+  </si>
+  <si>
+    <t>Kommunikation</t>
+  </si>
+  <si>
+    <t>Planung, Organisation</t>
+  </si>
+  <si>
+    <t>Visualisierung, Events</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +457,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -455,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -471,6 +524,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -14047,34 +14101,34 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
@@ -14082,12 +14136,12 @@
         <v>53</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -14106,7 +14160,7 @@
   <dimension ref="B1:W57"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14122,17 +14176,17 @@
     </row>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.25">
@@ -14140,13 +14194,13 @@
         <v>48</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.25">
@@ -14154,7 +14208,7 @@
         <v>49</v>
       </c>
       <c r="P7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.25">
@@ -14162,10 +14216,10 @@
         <v>50</v>
       </c>
       <c r="J8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.25">
@@ -14173,20 +14227,20 @@
         <v>51</v>
       </c>
       <c r="J9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M11" s="1"/>
     </row>
@@ -14195,79 +14249,100 @@
         <v>52</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="P15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F16" s="1"/>
       <c r="K16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
       <c r="Q25" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D27" s="7" t="s">
+        <v>135</v>
+      </c>
       <c r="Q27" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R27" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="S27" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="T27" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="T27" s="5" t="s">
+      <c r="U27" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="V27" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="U27" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="V27" s="5" t="s">
+      <c r="W27" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="W27" s="5" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="Q28" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R28" s="4">
         <v>18</v>
@@ -14286,9 +14361,19 @@
       </c>
       <c r="W28" s="4"/>
     </row>
-    <row r="33" spans="17:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="D31" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="4:23" x14ac:dyDescent="0.25">
       <c r="Q33" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R33" s="6"/>
       <c r="S33" s="6">
@@ -14307,59 +14392,64 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="17:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="4:23" x14ac:dyDescent="0.25">
       <c r="Q41" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="Q42" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="42" spans="17:23" x14ac:dyDescent="0.25">
-      <c r="Q42" t="s">
+    <row r="43" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="Q43" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="17:23" x14ac:dyDescent="0.25">
-      <c r="Q43" t="s">
+    <row r="44" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="Q44" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="17:23" x14ac:dyDescent="0.25">
-      <c r="Q44" t="s">
+    <row r="48" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="Q48" s="1" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="48" spans="17:23" x14ac:dyDescent="0.25">
-      <c r="Q48" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="49" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q49" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q50" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q51" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q55" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q56" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q57" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -14370,11 +14460,74 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C61D5E-3274-4E91-B4BA-CF516F62AFDD}">
+  <dimension ref="B3:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE61C21-B4DF-4ACF-89E3-F75BA53700E1}">
   <dimension ref="B2:N49"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I44" sqref="I44"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14387,10 +14540,10 @@
   <sheetData>
     <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N2" s="1"/>
     </row>
@@ -14399,7 +14552,7 @@
         <v>54</v>
       </c>
       <c r="L3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
@@ -14407,7 +14560,7 @@
         <v>55</v>
       </c>
       <c r="L4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.25">
@@ -14417,22 +14570,22 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.25">
@@ -14446,7 +14599,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57257774-D818-4A13-91F1-A7DCB0C009FC}">
   <dimension ref="B2:N63"/>
   <sheetViews>
@@ -14495,17 +14648,17 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -14572,7 +14725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47BD8981-4FF0-497D-829F-61801F8BAED6}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -14587,7 +14740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71006EA9-40F6-4D3A-95DF-25D6B75326D9}">
   <dimension ref="B2:J42"/>
   <sheetViews>
@@ -14750,7 +14903,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DACF6E-0F61-4744-BDED-4D535B825F26}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update Solutionkonzept und Systemvoraussetzungen
</commit_message>
<xml_diff>
--- a/8. Harmonising standards/Harmonizing SXI-DF.xlsx
+++ b/8. Harmonising standards/Harmonizing SXI-DF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\DataFactory-Knowledge-Center\8. Harmonising standards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBC38602-5529-4D0E-B58C-A933E74F4C23}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA4872A-F19D-429A-AB68-218CB97ADFC1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="4620" activeTab="1" xr2:uid="{16C57660-5F26-45F7-8E47-1B4877DEBD5B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="4620" activeTab="3" xr2:uid="{16C57660-5F26-45F7-8E47-1B4877DEBD5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Firmenmodell" sheetId="10" r:id="rId1"/>
@@ -21793,16 +21793,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>446276</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>34636</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>351026</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>181841</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>32306</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>45627</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>699056</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>2332</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -21817,8 +21817,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12027811" y="723034"/>
-          <a:ext cx="2634030" cy="1102037"/>
+          <a:off x="1260231" y="12330546"/>
+          <a:ext cx="2634030" cy="1153991"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -21866,50 +21866,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Solution</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" indent="0" algn="l"/>
-          <a:r>
-            <a:rPr lang="de-DE" sz="800" b="1">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>das Projekte professionell</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="de-DE" sz="800" b="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> umsetzen</a:t>
-          </a:r>
-          <a:endParaRPr lang="de-DE" sz="800" b="1">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
+            <a:t>MetaDaten</a:t>
+          </a:r>
         </a:p>
         <a:p>
           <a:pPr marL="0" indent="0" algn="l"/>
@@ -21939,7 +21897,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>basiert</a:t>
+            <a:t>Installierte Konnektoren</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="de-DE" sz="800" baseline="0">
@@ -21953,7 +21911,75 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> auf eine generischen Tabellenmodell</a:t>
+            <a:t> mit Name des Vorsystems</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Installierte Solutions</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Flag für Updatesteuerung </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Prozessflags (integrator import grad..)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Versionen (OCT, API, </a:t>
           </a:r>
           <a:endParaRPr lang="de-DE" sz="800">
             <a:solidFill>
@@ -21987,16 +22013,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>409641</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>163322</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>556846</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>59414</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>13987</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>11656</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>161192</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>98248</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -22011,8 +22037,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11991176" y="1942766"/>
-          <a:ext cx="2652346" cy="757538"/>
+          <a:off x="5276051" y="13160619"/>
+          <a:ext cx="2652346" cy="800834"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -22164,16 +22190,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>376669</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>11189</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>97781</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>646300</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>172382</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>31505</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>68474</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -22188,8 +22214,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11958204" y="3609042"/>
-          <a:ext cx="1793631" cy="1070397"/>
+          <a:off x="5243079" y="14913486"/>
+          <a:ext cx="1793631" cy="1113693"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -22452,16 +22478,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>405745</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>80195</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>552950</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>166787</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>10091</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>110369</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>157296</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>6461</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -22476,8 +22502,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11987280" y="2768843"/>
-          <a:ext cx="2652346" cy="757538"/>
+          <a:off x="5272155" y="14029992"/>
+          <a:ext cx="2652346" cy="792174"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -23850,8 +23876,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>493567</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>82261</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>173181</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -23866,8 +23892,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7050698" y="1203614"/>
-          <a:ext cx="1976404" cy="7386204"/>
+          <a:off x="7046368" y="1251239"/>
+          <a:ext cx="1976404" cy="7070147"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -24105,7 +24131,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> pro Person</a:t>
+            <a:t> pro Person incl. TZ Quote</a:t>
           </a:r>
           <a:endParaRPr lang="de-DE" sz="900" i="1">
             <a:solidFill>
@@ -24855,7 +24881,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Urlaub / Krankheit / Projekt</a:t>
+            <a:t>Urlaub / Krankheit / Projekt </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -25847,6 +25873,1974 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>290080</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>148071</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>287481</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>174048</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Rechteck 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76713C90-9224-4358-A141-12993011EB4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13391285" y="1438276"/>
+          <a:ext cx="1521401" cy="597477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Offene Posten</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Altersstruktur</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Abbau</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>156731</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>83993</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>154132</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>109970</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Rechteck 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44A0AB6F-A5E0-4748-A843-A4D96047D0A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11733936" y="2136198"/>
+          <a:ext cx="1521401" cy="597477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Fuhrpark</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Fahrzeugkosten</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>373540</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>5196</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>721570</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>16187</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Rechteck 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{847B89C7-ACCA-4690-BCAD-173A356353E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1282745" y="8153401"/>
+          <a:ext cx="2634030" cy="1153991"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+              <a:alpha val="25000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Dimension Kostenstellen</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Gruppierung</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> zu Profitcentern</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Fiktive Kostenstellen</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Hauptkostenstellen  / Hilfskostenstelle 1....X ter Ebene</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>378735</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>27710</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>726765</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>38701</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="Rechteck 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16111326-B08B-4DC7-B69B-CDAB96521DA0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1287940" y="9509415"/>
+          <a:ext cx="2634030" cy="1153991"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+              <a:alpha val="25000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Dimension Sachkonten</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Typ (Bilanz / GuV / Deb / Kred</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> )</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Fiktive Sachkonten (neu, für Umlage, Plankonto)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Exklusivität der Planung</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>130753</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>128154</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>187903</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="Rechteck 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BEC4F210-5341-45CD-9505-E804D01D4C78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11707958" y="1452131"/>
+          <a:ext cx="1521401" cy="597477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Umsatzplanung</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Artikelumsatz</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Kundenumsatz</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>352427</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>97848</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>349828</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="Rechteck 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{216D4D07-AAC0-45E0-ABBC-F726A8406A22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12691632" y="3483553"/>
+          <a:ext cx="1521401" cy="597477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Investitionsplanung</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Altersstruktur</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Abbau</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>158463</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>189635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>155864</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>25112</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="Rechteck 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCD2B9C4-7BFE-474C-A041-0B2201F1A2A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11735668" y="2813340"/>
+          <a:ext cx="1521401" cy="597477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Vertragsverwaltung</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Dauerschuldverhältnisse</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>345499</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>186172</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>21649</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="Rechteck 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA89A97F-629D-4CA8-BC28-E10E57BB9DFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12684704" y="4143377"/>
+          <a:ext cx="1521401" cy="597477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Darlehen</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Altersstruktur</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Abbau</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>563708</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>561109</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>187903</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="Rechteck 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F97888BC-359D-4FF3-A97F-273575D76847}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15188913" y="1452131"/>
+          <a:ext cx="1521401" cy="597477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Personaleinsatz</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Planung Person auf Projekt</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>264103</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>262370</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>562840</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>173181</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="Textfeld 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AF99F9E-D34F-484E-8EE3-7699E4D5B659}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11841308" y="452870"/>
+          <a:ext cx="1060737" cy="629516"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>Solutions</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t> mit</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1" baseline="0"/>
+            <a:t> Integration in GuV</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>537730</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>293543</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>74467</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>13854</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="Textfeld 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9C8B2D4-BEAA-4C5D-BCCB-76EDC98597D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15162935" y="484043"/>
+          <a:ext cx="1060737" cy="629516"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>Solutions</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t> ohne Finanz Integration</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>355889</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>284884</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>654626</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>5195</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="Textfeld 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08C2FE9C-6138-43BD-9107-B9AC851021FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13457094" y="475384"/>
+          <a:ext cx="1060737" cy="629516"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>Solutions</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1"/>
+            <a:t>mit</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" b="1" baseline="0"/>
+            <a:t> Integration in Liquidität</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>328181</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>325582</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="Rechteck 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A80B412-8C48-4EBD-9866-EA00C98917CF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13429386" y="4957331"/>
+          <a:ext cx="1521401" cy="731692"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>IFRS 16</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Bilanzierung von Leasingverträgen</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>49690</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>166255</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>510886</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>177246</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="Rechteck 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6008DE49-957F-4A41-9A73-23EAF24B9FD0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7054895" y="8504960"/>
+          <a:ext cx="1985196" cy="1153991"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+              <a:alpha val="25000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Dimension Person</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Name,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Geburtsdatum, Eintritt, Austritt</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>375272</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>32905</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>723302</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>43896</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="Rechteck 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CACC45C7-247A-4CEC-B67E-3CBF3D4887AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1284477" y="10848110"/>
+          <a:ext cx="2634030" cy="1153991"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+              <a:alpha val="25000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="36000" tIns="36000" rIns="36000" bIns="36000" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Dimension Mandanten</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="800">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Name, Gruppierung</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="800">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="50000"/>
+                <a:lumOff val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>662422</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>139412</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>659823</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>109104</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="67" name="Rechteck 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFE38301-5DD7-4337-B15B-79403C3BCBD6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9953627" y="6382617"/>
+          <a:ext cx="1521401" cy="731692"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Synchronisation</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Diff mit ToDo von System A und B</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>667618</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>49358</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>665019</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="68" name="Rechteck 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{375410DF-6D96-4145-A079-7F268C08F2B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9958823" y="7245063"/>
+          <a:ext cx="1521401" cy="731692"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Writeback</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="0" lang="de-DE" sz="900" b="0" i="1" u="none" strike="noStrike" kern="0" cap="none" spc="0" normalizeH="0" baseline="0" noProof="0">
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:solidFill>
+                <a:prstClr val="white">
+                  <a:lumMod val="75000"/>
+                </a:prstClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:uLnTx/>
+              <a:uFillTx/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Output Buchungen als CSV oder Systemformat</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
           <a:endParaRPr lang="de-DE" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -35552,22 +37546,22 @@
       <selection activeCell="T102" sqref="T102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" customWidth="1"/>
-    <col min="17" max="17" width="12.59765625" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="18" spans="13:17" x14ac:dyDescent="0.45">
+    <row r="18" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M18" s="1"/>
     </row>
-    <row r="30" spans="13:17" x14ac:dyDescent="0.45">
+    <row r="30" spans="13:17" x14ac:dyDescent="0.25">
       <c r="Q30" s="1"/>
     </row>
-    <row r="37" spans="17:17" x14ac:dyDescent="0.45">
+    <row r="37" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q37" s="1"/>
     </row>
-    <row r="44" spans="17:17" x14ac:dyDescent="0.45">
+    <row r="44" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q44" s="1"/>
     </row>
   </sheetData>
@@ -35581,49 +37575,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28EF74D8-9026-466E-B120-5AD0A17FB84D}">
   <dimension ref="G2:Q41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" customWidth="1"/>
-    <col min="17" max="17" width="12.59765625" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="7:13" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="7:13" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G2" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="7:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="7:13" x14ac:dyDescent="0.25">
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="7:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="7:13" x14ac:dyDescent="0.25">
       <c r="M10" s="1"/>
     </row>
-    <row r="11" spans="7:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="7:13" x14ac:dyDescent="0.25">
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="7:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="7:13" x14ac:dyDescent="0.25">
       <c r="M12" s="1"/>
     </row>
-    <row r="13" spans="7:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="7:13" x14ac:dyDescent="0.25">
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="7:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="7:13" x14ac:dyDescent="0.25">
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="7:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="7:13" x14ac:dyDescent="0.25">
       <c r="M15" s="1"/>
     </row>
-    <row r="27" spans="17:17" x14ac:dyDescent="0.45">
+    <row r="27" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q27" s="1"/>
     </row>
-    <row r="34" spans="17:17" x14ac:dyDescent="0.45">
+    <row r="34" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q34" s="1"/>
     </row>
-    <row r="41" spans="17:17" x14ac:dyDescent="0.45">
+    <row r="41" spans="17:17" x14ac:dyDescent="0.25">
       <c r="Q41" s="1"/>
     </row>
   </sheetData>
@@ -35641,7 +37635,7 @@
       <selection activeCell="R36" sqref="R36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -35652,16 +37646,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4FD98BF-1A98-47CF-A1FF-974E6BB79044}">
   <dimension ref="G2"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M38" sqref="M38"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="7:7" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="2" spans="7:7" ht="26.25" x14ac:dyDescent="0.4">
       <c r="G2" s="8" t="s">
         <v>138</v>
       </c>
@@ -35681,61 +37675,61 @@
       <selection activeCell="P47" sqref="P47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.1328125" customWidth="1"/>
-    <col min="17" max="17" width="12.59765625" customWidth="1"/>
+    <col min="1" max="1" width="2.140625" customWidth="1"/>
+    <col min="17" max="17" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="J6" s="1" t="s">
         <v>57</v>
       </c>
       <c r="P6" s="1"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J9" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J10" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>77</v>
       </c>
       <c r="M11" s="1"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
@@ -35746,7 +37740,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>50</v>
       </c>
@@ -35757,7 +37751,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>51</v>
       </c>
@@ -35769,7 +37763,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>52</v>
       </c>
@@ -35777,22 +37771,22 @@
         <v>56</v>
       </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="Q25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D27" s="7" t="s">
         <v>90</v>
       </c>
@@ -35818,7 +37812,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="Q28" s="4" t="s">
         <v>64</v>
       </c>
@@ -35839,17 +37833,17 @@
       </c>
       <c r="W28" s="4"/>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D31" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="33" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
         <v>49</v>
       </c>
@@ -35873,42 +37867,42 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="34" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D34" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="36" spans="4:23" x14ac:dyDescent="0.25">
       <c r="Q36" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="37" spans="4:23" x14ac:dyDescent="0.25">
       <c r="Q37" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="38" spans="4:23" x14ac:dyDescent="0.25">
       <c r="Q38" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="39" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="39" spans="4:23" x14ac:dyDescent="0.25">
       <c r="Q39" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="43" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="43" spans="4:23" x14ac:dyDescent="0.25">
       <c r="Q43" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="44" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="44" spans="4:23" x14ac:dyDescent="0.25">
       <c r="Q44" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="4:23" x14ac:dyDescent="0.45">
+    <row r="45" spans="4:23" x14ac:dyDescent="0.25">
       <c r="Q45" t="s">
         <v>87</v>
       </c>
@@ -35928,13 +37922,13 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="3.3984375" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>129</v>
       </c>
@@ -35942,12 +37936,12 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="N3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>94</v>
       </c>
@@ -35955,7 +37949,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>95</v>
       </c>
@@ -35963,12 +37957,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>97</v>
       </c>
@@ -35976,7 +37970,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>98</v>
       </c>
@@ -35984,7 +37978,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>99</v>
       </c>
@@ -35992,7 +37986,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>100</v>
       </c>
@@ -36000,7 +37994,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>101</v>
       </c>
@@ -36008,7 +38002,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>102</v>
       </c>
@@ -36016,7 +38010,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>103</v>
       </c>
@@ -36024,7 +38018,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>136</v>
       </c>
@@ -36032,73 +38026,73 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O16" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O17" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
       <c r="O18" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
       <c r="N20" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="M26" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B27" s="1"/>
       <c r="N27" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="N28" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="N29" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>109</v>
       </c>
@@ -36106,37 +38100,37 @@
         <v>135</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>130</v>
       </c>
@@ -36155,12 +38149,12 @@
       <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.86328125" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
@@ -36168,7 +38162,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -36176,7 +38170,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -36184,32 +38178,32 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N9" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="N11" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>0</v>
       </c>
@@ -36217,7 +38211,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>7</v>
       </c>
@@ -36225,7 +38219,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>8</v>
       </c>
@@ -36233,12 +38227,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>45</v>
       </c>
@@ -36252,7 +38246,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.45">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>44</v>
       </c>
@@ -36281,7 +38275,7 @@
       <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -36296,55 +38290,55 @@
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.3984375" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F4" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F5" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F6" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F7" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F8" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F9" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F10" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="F11" s="2"/>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>0</v>
       </c>
@@ -36352,7 +38346,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>37</v>
       </c>
@@ -36360,7 +38354,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -36368,7 +38362,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>42</v>
       </c>
@@ -36376,72 +38370,72 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>17</v>
       </c>

</xml_diff>